<commit_message>
adding the proportion dataset by mean and creating a plot to visualise
</commit_message>
<xml_diff>
--- a/PostWasting_PreWasting_Differences_20260117.xlsx
+++ b/PostWasting_PreWasting_Differences_20260117.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunoz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssaplayer/Desktop/AP-VRG-PVR-RefugiaAR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BA30BC72-7976-B145-857E-6D84ED34D4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A2981B-CAEA-2A45-9FD0-F3CFCA679C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2120" windowWidth="20900" windowHeight="13900" xr2:uid="{2B88350A-688B-394D-9B31-73924C2CF7D3}"/>
+    <workbookView xWindow="-20" yWindow="9320" windowWidth="15140" windowHeight="8700" xr2:uid="{2B88350A-688B-394D-9B31-73924C2CF7D3}"/>
   </bookViews>
   <sheets>
     <sheet name="PostWasting_PreWasting_Differen" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -92,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -650,7 +663,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -659,9 +672,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -1048,11 +1060,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC53CF96-F6F3-9C4C-8774-D459D1529388}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
@@ -1066,7 +1078,7 @@
     <col min="12" max="12" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="17" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1119,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1150,136 +1162,136 @@
         <v>4.1003346262239306</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>54.157674100000001</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>25.222353930000001</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>19.22043919</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>35.454545449999998</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>17.16856061</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>14.91385373</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>-34.937234910000001</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>-20.540691729999999</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>0.42</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <f t="shared" ref="L3:L21" si="0">1-G3/F3</f>
         <v>0.5157585468353536</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <f t="shared" ref="M3:M21" si="1">H3/G3</f>
         <v>0.86867234061038734</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>68.037339810000006</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>68.284279260000005</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>30.63780152</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>50.378787879999997</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>28.76173709</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>17.258371390000001</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>-37.399538290000002</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>-33.120416489999997</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>0.34</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f t="shared" si="0"/>
         <v>0.42909033146035269</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <f t="shared" si="1"/>
         <v>0.60004621195151886</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:13" ht="17" thickBot="1">
+      <c r="A5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>121.0827173</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>29.319918860000001</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>26.155763709999999</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>85.539772729999996</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <v>25.3125</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>16.254935140000001</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <v>-94.926953639999994</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="14">
         <v>-69.284837589999995</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="15">
         <v>0.19</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="16">
         <f t="shared" si="0"/>
         <v>0.70408502159694719</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <f t="shared" si="1"/>
         <v>0.64217027713580255</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1322,136 +1334,136 @@
         <v>2.7418028541750119</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>41.13949401</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>12.627201790000001</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>13.13370555</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>27.348484849999998</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>5.5208333329999997</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>4.7503516169999997</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>-28.005788460000002</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>-22.598133229999998</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <v>0.17</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <f t="shared" si="0"/>
         <v>0.79813019392918949</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <f t="shared" si="1"/>
         <v>0.86044104765949836</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>48.391694870000002</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>20.093406720000001</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>12.462180979999999</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>37.992424239999998</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>6.923076923</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>4.9915397629999996</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <v>-35.929513900000003</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="8">
         <v>-33.000884480000003</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>0.13</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <f t="shared" si="0"/>
         <v>0.8177774369104065</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="11">
         <f t="shared" si="1"/>
         <v>0.72100018799689991</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:13" ht="17" thickBot="1">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>39.009680410000001</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>9.1646210250000006</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>5.1239485629999999</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>30.4469697</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>2.6995305159999998</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>1.9577625569999999</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="14">
         <v>-33.885731849999999</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="14">
         <v>-28.489207140000001</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="15">
         <v>0.06</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="16">
         <f t="shared" si="0"/>
         <v>0.91133664392223568</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <f t="shared" si="1"/>
         <v>0.72522334731777482</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1494,136 +1506,136 @@
         <v>14.096085346092528</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>9.5685131509999994</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.37154211199999998</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>0.66406726000000005</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>7.8030303029999999</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>6.6287878999999994E-2</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>0.233825598</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <v>-8.9044458909999999</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>-7.5692047049999998</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>0.03</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <f t="shared" si="0"/>
         <v>0.99150485434171454</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="11">
         <f t="shared" si="1"/>
         <v>3.5274261528265223</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>14.489170489999999</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>0.36600603500000001</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>0.98124767300000004</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>15.31060606</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>5.8685446000000002E-2</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>0.31202435299999998</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>-13.507922819999999</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <v>-14.99858171</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>0.02</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <f t="shared" si="0"/>
         <v>0.99616700699044702</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="11">
         <f t="shared" si="1"/>
         <v>5.3168949759707029</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:13" ht="17" thickBot="1">
+      <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>16.004948280000001</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>0.324085134</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>0.833980744</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>17.48106061</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <v>4.8076923000000001E-2</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>0.26790750099999999</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="14">
         <v>-15.17096753</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="14">
         <v>-17.2131531</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="15">
         <v>0.02</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="16">
         <f t="shared" si="0"/>
         <v>0.9972497708192547</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <f t="shared" si="1"/>
         <v>5.5724760297159612</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1663,133 +1675,133 @@
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>7.2301634879999996</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>0.32216178899999998</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>0.57903003799999997</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>4.8181818180000002</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>6.4553991000000005E-2</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>0.11796042599999999</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <v>-6.6511334499999997</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <v>-4.7002213920000004</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="9">
         <v>0.02</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <f t="shared" si="0"/>
         <v>0.98660200186741898</v>
       </c>
-      <c r="M15" s="12">
+      <c r="M15" s="11">
         <f t="shared" si="1"/>
         <v>1.8273142244605758</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>5.4021346770000003</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>0</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>0.17036132600000001</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>1.4610389610000001</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <v>0</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <v>1.7580872000000001E-2</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="8">
         <v>-5.2317733510000002</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="8">
         <v>-1.4434580889999999</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="9">
         <v>0.01</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M16" s="12"/>
+      <c r="M16" s="11"/>
     </row>
-    <row r="17" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:13" ht="17" thickBot="1">
+      <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>9.8120688709999992</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>1.5234644020000001</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>0.26235290300000003</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>6.7613636359999996</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="14">
         <v>0.23237179499999999</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <v>4.2301183999999999E-2</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="14">
         <v>-9.5497159679999992</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="14">
         <v>-6.7190624520000002</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="15">
         <v>0.01</v>
       </c>
-      <c r="L17" s="17">
+      <c r="L17" s="16">
         <f t="shared" si="0"/>
         <v>0.96563240678806761</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="17">
         <f t="shared" si="1"/>
         <v>0.18204095725128774</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1832,131 +1844,131 @@
         <v>2.0748838891730612</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>927.61042380000004</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>332.44847729999998</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>187.51798579999999</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>531.82575759999997</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>124.67722999999999</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>72.393455099999997</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <v>-740.09243809999998</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <v>-459.43230249999999</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="10">
         <f t="shared" si="0"/>
         <v>0.76556752241065207</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="11">
         <f t="shared" si="1"/>
         <v>0.58064696416498829</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>432.22094929999997</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>170.96964070000001</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>46.545186610000002</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>190.91991340000001</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>44.403409089999997</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>19.229957809999998</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>-385.67576270000001</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>-171.68995559999999</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>0.1</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="10">
         <f t="shared" si="0"/>
         <v>0.76742389885244944</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="11">
         <f t="shared" si="1"/>
         <v>0.43307390590266048</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:13" ht="17" thickBot="1">
+      <c r="A21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>372.63651429999999</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <v>220.62544349999999</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>38.347918909999997</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <v>289.72537879999999</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="14">
         <v>62.01923077</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>21.00394811</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="14">
         <v>-334.28859540000002</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="14">
         <v>-268.72143069999998</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="16">
         <f t="shared" si="0"/>
         <v>0.78593787321333552</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="17">
         <f t="shared" si="1"/>
         <v>0.33866831060665215</v>
       </c>
@@ -1964,6 +1976,18 @@
   </sheetData>
   <conditionalFormatting sqref="K2:K5">
     <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K21">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2012,6 +2036,134 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:K21">
     <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L5">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L21">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6:L9">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10:L13">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14:L17">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18:L21">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M21">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2082,146 +2234,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L5">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L6:L9">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L10:L13">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L12">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L10">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L14:L17">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L18:L21">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K21">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M21">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L21">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>